<commit_message>
angepasst: hier und im FDZ-Allgemein\Codierlisten
</commit_message>
<xml_diff>
--- a/data/instruments/attachments/cl-dzhw-6.xlsx
+++ b/data/instruments/attachments/cl-dzhw-6.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Code</t>
   </si>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,30 +639,6 @@
         <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>